<commit_message>
PEGA Chnage request code is pushed
</commit_message>
<xml_diff>
--- a/HFIC/TestData/TestData.xlsx
+++ b/HFIC/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F5192-506A-405D-8F09-7AEFEEFC412A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75E6D86-7366-4344-9893-0B05B9634DBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>srikanth@get365.tk</t>
   </si>
@@ -32,100 +32,100 @@
     <t>Passw0rd#12</t>
   </si>
   <si>
-    <t>1/1/2018</t>
-  </si>
-  <si>
-    <t>'1/1/2018</t>
-  </si>
-  <si>
-    <t>CG0399</t>
-  </si>
-  <si>
-    <t>HARMONY HEIGHTS INC</t>
-  </si>
-  <si>
-    <t>CG0398</t>
-  </si>
-  <si>
-    <t>OEM SOURCE INC</t>
-  </si>
-  <si>
-    <t>CG0397</t>
-  </si>
-  <si>
-    <t>SIMPLY CLEAN</t>
-  </si>
-  <si>
-    <t>CG0396</t>
-  </si>
-  <si>
-    <t>MICHAEL D WILDER CPA</t>
-  </si>
-  <si>
-    <t>CG0395</t>
-  </si>
-  <si>
-    <t>TAXPERTS OF NY INC.</t>
-  </si>
-  <si>
-    <t>CG0394</t>
-  </si>
-  <si>
-    <t>DASTECH INTERNATIONAL, INC.</t>
-  </si>
-  <si>
-    <t>SAFETY FIRST ARMED COURIER</t>
-  </si>
-  <si>
-    <t>CG0392</t>
-  </si>
-  <si>
-    <t>ORTHOPEDIC ALTERNATIVES INC</t>
-  </si>
-  <si>
-    <t>CG0391</t>
-  </si>
-  <si>
-    <t>CHARLES PFEIFFER INC</t>
-  </si>
-  <si>
-    <t>CG0390</t>
-  </si>
-  <si>
-    <t>GRIP COLLECTIONS INC</t>
-  </si>
-  <si>
-    <t>CG0393</t>
-  </si>
-  <si>
-    <t>237338682</t>
-  </si>
-  <si>
-    <t>651276620</t>
-  </si>
-  <si>
-    <t>113496553</t>
-  </si>
-  <si>
-    <t>274613643</t>
-  </si>
-  <si>
-    <t>112576892</t>
-  </si>
-  <si>
-    <t>133032912</t>
-  </si>
-  <si>
-    <t>113058008</t>
-  </si>
-  <si>
-    <t>112869106</t>
-  </si>
-  <si>
-    <t>132887066</t>
-  </si>
-  <si>
-    <t>205834290</t>
+    <t>CG0499</t>
+  </si>
+  <si>
+    <t>IDEAL FOOT CARE PC</t>
+  </si>
+  <si>
+    <t>CG0498</t>
+  </si>
+  <si>
+    <t>CLINTON ARMS ASSOCIATES</t>
+  </si>
+  <si>
+    <t>CG0497</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL EXPERIENCE</t>
+  </si>
+  <si>
+    <t>CG0496</t>
+  </si>
+  <si>
+    <t>ENGINEERING GROUP ASSOC P.C</t>
+  </si>
+  <si>
+    <t>CG0495</t>
+  </si>
+  <si>
+    <t>H.W. ANDERSON CONSULTING, INC.</t>
+  </si>
+  <si>
+    <t>CG0494</t>
+  </si>
+  <si>
+    <t>GREENE AVENUE ASSOCIATES</t>
+  </si>
+  <si>
+    <t>CG0493</t>
+  </si>
+  <si>
+    <t>EAST 168TH STREET ASSOCIATES</t>
+  </si>
+  <si>
+    <t>CG0492</t>
+  </si>
+  <si>
+    <t>LAW OFFICE OF WILLIAM J MCDER</t>
+  </si>
+  <si>
+    <t>CG0491</t>
+  </si>
+  <si>
+    <t>JEWISH COMM PROJ OF LWR MANHAT</t>
+  </si>
+  <si>
+    <t>CG0490</t>
+  </si>
+  <si>
+    <t>S&amp;K WARBASSE PHARMACY</t>
+  </si>
+  <si>
+    <t>01/01/2018</t>
+  </si>
+  <si>
+    <t>464638837</t>
+  </si>
+  <si>
+    <t>112676441</t>
+  </si>
+  <si>
+    <t>112480497</t>
+  </si>
+  <si>
+    <t>272346235</t>
+  </si>
+  <si>
+    <t>352523812</t>
+  </si>
+  <si>
+    <t>112604693</t>
+  </si>
+  <si>
+    <t>112676440</t>
+  </si>
+  <si>
+    <t>113399299</t>
+  </si>
+  <si>
+    <t>113706587</t>
+  </si>
+  <si>
+    <t>208799775</t>
+  </si>
+  <si>
+    <t>Change request Uplode document General notes</t>
   </si>
 </sst>
 </file>
@@ -528,157 +528,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9684E98A-EA7A-41F6-A6B8-842EDFAC86CC}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CR Upload documents -4/4
</commit_message>
<xml_diff>
--- a/HFIC/TestData/TestData.xlsx
+++ b/HFIC/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75E6D86-7366-4344-9893-0B05B9634DBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3D192-03DD-454D-AA93-186CA7ECE840}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>srikanth@get365.tk</t>
   </si>
@@ -125,7 +125,10 @@
     <t>208799775</t>
   </si>
   <si>
-    <t>Change request Uplode document General notes</t>
+    <t>Change request Upload document General notes</t>
+  </si>
+  <si>
+    <t>Other Supporting documents</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9684E98A-EA7A-41F6-A6B8-842EDFAC86CC}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G1" sqref="G1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +542,11 @@
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -558,8 +562,11 @@
       <c r="F1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -572,8 +579,14 @@
       <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -586,8 +599,14 @@
       <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -600,8 +619,14 @@
       <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -614,8 +639,14 @@
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -628,8 +659,14 @@
       <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -642,8 +679,14 @@
       <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -656,8 +699,14 @@
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -670,8 +719,14 @@
       <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -683,6 +738,12 @@
       </c>
       <c r="D10" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HSA and upload document completed
</commit_message>
<xml_diff>
--- a/HFIC/TestData/TestData.xlsx
+++ b/HFIC/TestData/TestData.xlsx
@@ -3,14 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3D192-03DD-454D-AA93-186CA7ECE840}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505BDE4A-FAD6-477D-8AA2-FC6AA01AB3D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFIC" sheetId="1" r:id="rId1"/>
     <sheet name="CR" sheetId="2" r:id="rId2"/>
+    <sheet name="HSA" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">HSA!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
   <si>
     <t>srikanth@get365.tk</t>
   </si>
@@ -129,6 +134,207 @@
   </si>
   <si>
     <t>Other Supporting documents</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC1JULY10244</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY547</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY965</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY617</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY295</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY757</t>
+  </si>
+  <si>
+    <t>TESTINGGTMC2JULY635</t>
+  </si>
+  <si>
+    <t>666705335</t>
+  </si>
+  <si>
+    <t>323235236</t>
+  </si>
+  <si>
+    <t>222164623</t>
+  </si>
+  <si>
+    <t>272733349</t>
+  </si>
+  <si>
+    <t>151542333</t>
+  </si>
+  <si>
+    <t>201985161</t>
+  </si>
+  <si>
+    <t>878811382</t>
+  </si>
+  <si>
+    <t>Contact perdon update</t>
+  </si>
+  <si>
+    <t>Sand creek road</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>12206</t>
+  </si>
+  <si>
+    <t>8905671234</t>
+  </si>
+  <si>
+    <t>Grpupdate@HSA.COM</t>
+  </si>
+  <si>
+    <t>lname_update</t>
+  </si>
+  <si>
+    <t>fname_Update</t>
+  </si>
+  <si>
+    <t>01/01/1981</t>
+  </si>
+  <si>
+    <t>678345891</t>
+  </si>
+  <si>
+    <t>driver 1234</t>
+  </si>
+  <si>
+    <t>12202</t>
+  </si>
+  <si>
+    <t>"HSA Notes : Member details has been successfully  updated</t>
+  </si>
+  <si>
+    <t>HSA Notes : Group details are updated successfully</t>
+  </si>
+  <si>
+    <t>Sand creek road 12</t>
+  </si>
+  <si>
+    <t>RIDGARD391</t>
+  </si>
+  <si>
+    <t>MENTON</t>
+  </si>
+  <si>
+    <t>MCENTEE610</t>
+  </si>
+  <si>
+    <t>JESSY</t>
+  </si>
+  <si>
+    <t>JEM</t>
+  </si>
+  <si>
+    <t>JAZ</t>
+  </si>
+  <si>
+    <t>JIN</t>
+  </si>
+  <si>
+    <t>JANW</t>
+  </si>
+  <si>
+    <t>FNAMEUPDATE</t>
+  </si>
+  <si>
+    <t>LNAMEUPDATE</t>
+  </si>
+  <si>
+    <t>RANI</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>45012514500</t>
+  </si>
+  <si>
+    <t>45012514400</t>
+  </si>
+  <si>
+    <t>45012514300</t>
+  </si>
+  <si>
+    <t>45012513900</t>
+  </si>
+  <si>
+    <t>45012513600</t>
+  </si>
+  <si>
+    <t>45012513800</t>
+  </si>
+  <si>
+    <t>45012513100</t>
+  </si>
+  <si>
+    <t>45012513300</t>
+  </si>
+  <si>
+    <t>45012513200</t>
+  </si>
+  <si>
+    <t>45012497200</t>
+  </si>
+  <si>
+    <t>45012497100</t>
+  </si>
+  <si>
+    <t>45012497000</t>
+  </si>
+  <si>
+    <t>45012496900</t>
+  </si>
+  <si>
+    <t>CG5012</t>
+  </si>
+  <si>
+    <t>CG5011</t>
+  </si>
+  <si>
+    <t>CG5010</t>
+  </si>
+  <si>
+    <t>CG5008</t>
+  </si>
+  <si>
+    <t>CG5007</t>
+  </si>
+  <si>
+    <t>CG5006</t>
+  </si>
+  <si>
+    <t>CG5004</t>
+  </si>
+  <si>
+    <t>CG5003</t>
+  </si>
+  <si>
+    <t>CG5001</t>
+  </si>
+  <si>
+    <t>CG5000</t>
+  </si>
+  <si>
+    <t>CG4998</t>
+  </si>
+  <si>
+    <t>CG4997</t>
   </si>
 </sst>
 </file>
@@ -172,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -195,12 +401,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -212,6 +427,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9684E98A-EA7A-41F6-A6B8-842EDFAC86CC}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,4 +971,343 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429E2D65-46FC-4E21-9DB5-EB567EC510F0}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E06FC4A3-CF87-4C6E-8D77-7DC31AD6245D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>